<commit_message>
Remove outdated image and update Excel output; enhance process_image.py with new functions and improved error handling; add comprehensive documentation in memory-bank files.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>268   444   6   86   8   26   86   8   28   6   8   2K   2</t>
+          <t>268 444 6 86 8 26 86 8 28 6 8 2K 2</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -503,7 +503,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$  386  ,  523  ,  434  ,  322.15 AND 26 %</t>
+          <t>$ 386 , 523 , 434 , 322.15 AND 26 %</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -518,22 +518,22 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>6E   8   2   4   8   2   6   8   6   2   6   8</t>
+          <t>6E 8 2 4 8  2 6 8 6 2 6 8</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>$  286  ,  027  ,  341  ,  398.39 AND $  1  ,  316  ,  707  ,  236.80</t>
+          <t>$ 286 , 027 , 341 , 398.39 AND $ 1 , 305 , 350 , 268.83</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>$  0.00 AND $  42  ,  595  ,  191  ,  764.52</t>
+          <t>$ 0.00 AND $ 42 , 595 , 191 , 764.52</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>$  76  ,  273  ,  957.85 AND NA</t>
+          <t>$ 76 , 273 , 957.85 AND NA</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor data extraction in parse_and_transform_data; update field types to numbers and simplify logic for improved clarity and performance.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -503,12 +503,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$ 386 , 523 , 434 , 322.15 AND 26 %</t>
+          <t>$ 38 , 656 , 710 , 449 , 061.55 AND 26 %</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>17 YEARS AND 0.00 %</t>
+          <t>17 YEARS AND 16.30 %</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -523,12 +523,12 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>$ 286 , 027 , 341 , 398.39 AND $ 1 , 305 , 350 , 268.83</t>
+          <t>$ 28 , 605 , 965 , 732 , 305.55 AND $ 131 , 685 , 600 , 094.16</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>$ 0.00 AND $ 42 , 595 , 191 , 764.52</t>
+          <t>$ 67 , 186 , 820 , 273 , 079.76 AND $ 42 , 595 , 191 , 764.52</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">

</xml_diff>